<commit_message>
Recognise custom date formats, and drop support for TimeSpan
It is only possible to recognise a date value in excel from the number
format, which is utterly idiotic. Previously the code only recognised
built in date formats, but now it should support most custom formats
as well, although when round tripping for format will revert to a built
in one.

TimeSpan is very csharp specific, and thinking about extending this to
python. Its also easy to convert from a date time to a time span
yourself, so the framework isn't really adding much.
</commit_message>
<xml_diff>
--- a/Test/TestExcelFiles/PropertyTypes.xlsx
+++ b/Test/TestExcelFiles/PropertyTypes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\Test\TestExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E2E50A5A-E9B1-42A9-8A06-1EA5D0BA7D29}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3AA74B-33C3-4E50-9730-129D4B073726}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
   </bookViews>
   <sheets>
     <sheet name="AllPropertyTypes" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Specification</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>DateTime of</t>
-  </si>
-  <si>
-    <t>TimeSpan of</t>
   </si>
   <si>
     <t>null</t>
@@ -141,15 +138,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -570,26 +564,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1389079D-C9FD-4AFA-AFB3-2F9AFFAD165C}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" style="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="12.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,7 +591,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -605,25 +599,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
@@ -631,91 +625,83 @@
         <v>43466</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="3">
-        <v>5.2083333333333336E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>